<commit_message>
Updates in Project Selection File
Minor updates to Excel project selection file.
</commit_message>
<xml_diff>
--- a/CandidateProjects/ProjectSelection.xlsx
+++ b/CandidateProjects/ProjectSelection.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isral\Documents\GitHub\MSAAI501\CandidateProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA855BFA-C3F4-4F10-A625-0FCC716BA012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1A2800-831F-4732-B718-A8C9A44F7A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD74D771-89FF-4C58-8CFC-27B83C20845C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{CD74D771-89FF-4C58-8CFC-27B83C20845C}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSelection" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Dataset</t>
   </si>
@@ -63,9 +64,6 @@
   </si>
   <si>
     <t>1 - Phishing Identification - Israel</t>
-  </si>
-  <si>
-    <t>Discarded</t>
   </si>
   <si>
     <t>235k</t>
@@ -151,9 +149,6 @@
 Understanding the variables might delay us</t>
   </si>
   <si>
-    <t>Might be complex enough to fill 20-30 min</t>
-  </si>
-  <si>
     <t>Very straight forward
 No background story to describe</t>
   </si>
@@ -175,9 +170,6 @@
   <si>
     <t>Very straight forward
 Pricing is easy to work with</t>
-  </si>
-  <si>
-    <t>Challenging Algorithm Selection</t>
   </si>
   <si>
     <t>Very interesting and new
@@ -193,9 +185,6 @@
 Not a lot of pre-processing</t>
   </si>
   <si>
-    <t>Not as interesting to build?</t>
-  </si>
-  <si>
     <t>Too Alex dependent - requirement of previous knowledge of the protocols</t>
   </si>
   <si>
@@ -221,6 +210,98 @@
   </si>
   <si>
     <t>Not too attractive</t>
+  </si>
+  <si>
+    <t>Not as interesting to build?
+Not clear what we can predict with the available data</t>
+  </si>
+  <si>
+    <t>Might be complex enough to fill 20-30 min
+A lot of work available around it</t>
+  </si>
+  <si>
+    <t>Finalist</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Standardized Values</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Booleans</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>family_history_with_overweight, FAVC, SMOKE, SCC</t>
+  </si>
+  <si>
+    <t>CAEC, CALC</t>
+  </si>
+  <si>
+    <t>Sometimes</t>
+  </si>
+  <si>
+    <t>Frequently</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>MTRANS</t>
+  </si>
+  <si>
+    <t>Public_Transportation</t>
+  </si>
+  <si>
+    <t>Walking</t>
+  </si>
+  <si>
+    <t>Automobile</t>
+  </si>
+  <si>
+    <t>Motorbike</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>NObeyesdad</t>
+  </si>
+  <si>
+    <t>Normal_Weight</t>
+  </si>
+  <si>
+    <t>Overweight_Level_I</t>
+  </si>
+  <si>
+    <t>Overweight_Level_II</t>
+  </si>
+  <si>
+    <t>Obesity_Type_I</t>
+  </si>
+  <si>
+    <t>Insufficient_Weight</t>
+  </si>
+  <si>
+    <t>Obesity_Type_II</t>
+  </si>
+  <si>
+    <t>Obesity_Type_III</t>
   </si>
 </sst>
 </file>
@@ -242,12 +323,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -347,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -355,7 +442,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,6 +455,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -393,15 +489,450 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FFA3A3A3"/>
         </left>
         <right style="medium">
           <color rgb="FFA3A3A3"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFA3A3A3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FFA3A3A3"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFA3A3A3"/>
+        </right>
+        <bottom style="medium">
+          <color rgb="FFA3A3A3"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -441,450 +972,15 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color rgb="FFA3A3A3"/>
         </left>
         <right style="medium">
           <color rgb="FFA3A3A3"/>
         </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFA3A3A3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FFA3A3A3"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFA3A3A3"/>
-        </right>
-        <bottom style="medium">
-          <color rgb="FFA3A3A3"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -901,24 +997,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6909FEF0-3E9D-4B75-9238-B17A84AE6001}" name="Table1" displayName="Table1" ref="A1:M11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6909FEF0-3E9D-4B75-9238-B17A84AE6001}" name="Table1" displayName="Table1" ref="A1:M11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A1:M11" xr:uid="{6909FEF0-3E9D-4B75-9238-B17A84AE6001}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M11">
+    <sortCondition descending="1" ref="B2:B11"/>
+  </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{26973439-535B-4950-A529-1646FA351911}" name="Dataset" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{ECB1981D-2AB0-4DCF-9486-680FD28A4796}" name="Ranking" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{26973439-535B-4950-A529-1646FA351911}" name="Dataset" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{ECB1981D-2AB0-4DCF-9486-680FD28A4796}" name="Ranking" dataDxfId="11">
       <calculatedColumnFormula>E2+G2+I2+K2+M2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B6EAFA7A-8F15-4B2A-9817-A1C7C359973F}" name="Decision" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{4FA550C0-3AB2-43CB-A397-8C3104A5E90E}" name="No. Records" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{0CB29568-6662-48DE-9DE0-E75C09D8FA7C}" name="Rec Points" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{E965737F-64B6-44CA-9A51-8FAAEC03378D}" name="Type" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{E66CC76E-9109-49A4-8AE0-23C588ABE98C}" name="Type Points" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{3D61590E-E47F-4D2E-8CFA-AA5C6E9F66C8}" name="Pros" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{80CFAC36-7F7A-4FC2-BF51-8C37071F29A9}" name="Pro Points" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{35B90B85-EC75-4F5D-961C-6FCEE1A801ED}" name="Cons" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{83C405F6-8D48-4292-A986-026592A127EC}" name="Cons Points" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{34E27A8D-6D5B-4B91-AC55-02E43EE20ACC}" name="Difficulty" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{A95B42DC-6663-4DF3-9221-7B739A2A414B}" name="Diff Points" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B6EAFA7A-8F15-4B2A-9817-A1C7C359973F}" name="Decision" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{4FA550C0-3AB2-43CB-A397-8C3104A5E90E}" name="No. Records" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{0CB29568-6662-48DE-9DE0-E75C09D8FA7C}" name="Rec Points" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E965737F-64B6-44CA-9A51-8FAAEC03378D}" name="Type" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{E66CC76E-9109-49A4-8AE0-23C588ABE98C}" name="Type Points" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{3D61590E-E47F-4D2E-8CFA-AA5C6E9F66C8}" name="Pros" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{80CFAC36-7F7A-4FC2-BF51-8C37071F29A9}" name="Pro Points" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{35B90B85-EC75-4F5D-961C-6FCEE1A801ED}" name="Cons" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{83C405F6-8D48-4292-A986-026592A127EC}" name="Cons Points" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{34E27A8D-6D5B-4B91-AC55-02E43EE20ACC}" name="Difficulty" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{A95B42DC-6663-4DF3-9221-7B739A2A414B}" name="Diff Points" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1243,11 +1342,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAA9E95-ABD9-42A7-9682-9FB9887DAA7D}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="63.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,58 +1380,56 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <f>E2+G2+I2+K2+M2</f>
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <f t="shared" ref="B2:B11" si="0">E2+G2+I2+K2+M2</f>
         <v>9</v>
       </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1">
         <v>2</v>
@@ -1341,174 +1438,170 @@
         <v>36</v>
       </c>
       <c r="K2" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M2" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
-        <f>E3+G3+I3+K3+M3</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G3" s="1">
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I3" s="1">
         <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="K3" s="1">
         <v>-1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M3" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1">
-        <f>E4+G4+I4+K4+M4</f>
-        <v>7</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="9">
+        <v>3</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1">
+      <c r="M4" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="J5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1">
-        <f>E5+G5+I5+K5+M5</f>
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="1">
-        <v>-3</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
-        <f>E6+G6+I6+K6+M6</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1">
         <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="I6" s="1">
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="K6" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M6" s="4">
         <v>2</v>
@@ -1516,196 +1609,194 @@
     </row>
     <row r="7" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
-        <f>E7+G7+I7+K7+M7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1">
         <v>-2</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M7" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
-        <f>E8+G8+I8+K8+M8</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K8" s="1">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
-        <f>E9+G9+I9+K9+M9</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
       <c r="J9" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="K9" s="1">
         <v>-3</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M9" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
-        <f>E10+G10+I10+K10+M10</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1">
-        <v>3</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="K10" s="1">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6">
-        <f>E11+G11+I11+K11+M11</f>
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>14</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="6">
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G11" s="6">
-        <v>4</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="6">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="K11" s="6">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M11" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1747,4 +1838,217 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1850A058-F76B-4AF5-A58B-35055CADC540}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G15:H21">
+    <sortCondition ref="H15:H21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>